<commit_message>
Add Jobs, eons, demons, status, items, refacto des skills et des spells
</commit_message>
<xml_diff>
--- a/MyJDR_Calc.xlsx
+++ b/MyJDR_Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://settis-my.sharepoint.com/personal/alexandre_receveur_alliance4u_fr/Documents/Documents/JDR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4758" documentId="11_9248CACD84F5E813E97046798E3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2FCB9F4-9BAC-486E-9F52-62D3FB54B607}"/>
+  <xr:revisionPtr revIDLastSave="4759" documentId="11_9248CACD84F5E813E97046798E3E8C1851038385" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D2BD496-E938-40AB-AEBB-A150EF14F510}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5159,8 +5159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBB7AAE-1E9E-4FCF-92CB-4B50C269FA39}">
   <dimension ref="A1:AF187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M8" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -5194,7 +5194,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C1" s="62"/>
       <c r="D1" s="62"/>
@@ -5733,7 +5733,7 @@
 _xlpm.sort,_xlfn.XLOOKUP(G7,Magies!$B$2:$B$40,Magies!$E$2:$E$40),
 _xlpm.calcul,IF(_xlpm.roll&gt;1,IF(_xlpm.roll&gt;=(_xlpm.sort-F13),
 (((F13+_xlpm.sort)^2)/2*_xlpm.faiblesse)+_xlpm.roll+$F$2,0)*IF(_xlpm.roll=6,_xlpm.crit,1),"Fumble"),IFERROR(ROUNDDOWN(_xlpm.calcul,0),_xlpm.calcul)),IF(AND(G6="Magie",_xlfn.XLOOKUP(G7,Magies!$B$2:$B$40,Magies!$A$2:$A$40)="Allié"),_xlfn.CONCAT("Soin ",_xlfn.XLOOKUP(G7,Magies!$B$2:$B$40,Magies!$F$2:$F$40),"PV"),"Erreur Magie")))),"Erreur"))</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H10" s="62"/>
       <c r="I10" s="81"/>
@@ -5770,7 +5770,7 @@
 _xlpm.sort,_xlfn.XLOOKUP(M7,Magies!$B$2:$B$40,Magies!$E$2:$E$40),
 _xlpm.calcul,IF(_xlpm.roll&gt;1,IF(_xlpm.roll&gt;=(_xlpm.sort-L13),
 (((L13+_xlpm.sort)^2)/2*_xlpm.faiblesse)+_xlpm.roll+$F$2,0)*IF(_xlpm.roll=6,_xlpm.crit,1),"Fumble"),IFERROR(ROUNDDOWN(_xlpm.calcul,0),_xlpm.calcul)),IF(AND(M6="Magie",_xlfn.XLOOKUP(M7,Magies!$B$2:$B$40,Magies!$A$2:$A$40)="Allié"),_xlfn.CONCAT("Soin ",_xlfn.XLOOKUP(M7,Magies!$B$2:$B$40,Magies!$F$2:$F$40),"PV"),"Erreur Magie")))),"Erreur"))</f>
-        <v>1950</v>
+        <v>324</v>
       </c>
       <c r="N10" s="63"/>
       <c r="O10" s="82"/>
@@ -5808,7 +5808,7 @@
 _xlpm.calcul,IF(_xlpm.roll&gt;1,IF(_xlpm.roll&gt;=(_xlpm.sort-R13),
 (((R13+_xlpm.sort)^2)/2*_xlpm.faiblesse)+_xlpm.roll+$F$2,0)*IF(_xlpm.roll=6,_xlpm.crit,1),"Fumble"),
 IFERROR(ROUNDDOWN(_xlpm.calcul,0),_xlpm.calcul)),IF(AND(S6="Magie",_xlfn.XLOOKUP(S7,Magies!$B$2:$B$40,Magies!$A$2:$A$40)="Allié"),_xlfn.CONCAT("Soin ",_xlfn.XLOOKUP(S7,Magies!$B$2:$B$40,Magies!$F$2:$F$40),"PV"),"Erreur Magie")))),"Erreur"))</f>
-        <v>816</v>
+        <v>135</v>
       </c>
       <c r="T10" s="62"/>
       <c r="U10" s="63"/>
@@ -5845,7 +5845,7 @@
 ((W13+_xlpm.sort)*_xlpm.faiblesse),0)+IF(_xlpm.roll=6,_xlpm.crit+5,0)*_xlpm.faiblesse,"Fumble"),_xlpm.calcul),
 IF(AND(X6="Magie",_xlfn.XLOOKUP(X7,Magies!$B$2:$B$40,Magies!$A$2:$A$40)="Allié"),
 _xlfn.CONCAT("Soin ",_xlfn.XLOOKUP(X7,Magies!$B$2:$B$40,Magies!$F$2:$F$40),"PV"),"Erreur Magie")))),"Erreur"))</f>
-        <v>864</v>
+        <v>135</v>
       </c>
       <c r="Y10" s="62"/>
       <c r="Z10" s="62"/>
@@ -6353,7 +6353,7 @@
       </c>
       <c r="N22" s="79">
         <f ca="1">IFERROR(M22-(IF(ISNUMBER(G10),G10,0)+IF(ISNUMBER(M10),M10,0)+IF(ISNUMBER(S10),S10,0)+IF(ISNUMBER(X10),X10,0)),"")</f>
-        <v>-3175</v>
+        <v>-126</v>
       </c>
       <c r="O22" s="156" cm="1">
         <f t="array" aca="1" ref="O22" ca="1">IFERROR(INDIRECT(_xlfn.CONCAT("'Bestiaire'!",ADDRESS(ROW(_xlfn.XLOOKUP(Equipe!L22,Bestiaire!$C$4:$C$35,Bestiaire!$C$4:$C$35)),11+3*($N$1-1)))),"")</f>
@@ -6459,7 +6459,7 @@
       </c>
       <c r="N24" s="79">
         <f t="shared" ca="1" si="0"/>
-        <v>-750</v>
+        <v>876</v>
       </c>
       <c r="O24" s="156" cm="1">
         <f t="array" aca="1" ref="O24" ca="1">IFERROR(INDIRECT(_xlfn.CONCAT("'Bestiaire'!",ADDRESS(ROW(_xlfn.XLOOKUP(Equipe!L24,Bestiaire!$C$4:$C$35,Bestiaire!$C$4:$C$35)),11+3*($N$1-1)))),"")</f>
@@ -6559,7 +6559,7 @@
 ((W28+_xlpm.sort)*_xlpm.faiblesse),0)+IF(_xlpm.roll=6,_xlpm.crit+5,0)*_xlpm.faiblesse,"Fumble"),_xlpm.calcul),
 IF(AND(X21="Magie",_xlfn.XLOOKUP(X22,Magies!$B$2:$B$40,Magies!$A$2:$A$40)="Allié"),
 _xlfn.CONCAT("Soin ",_xlfn.XLOOKUP(X22,Magies!$B$2:$B$40,Magies!$F$2:$F$40),"PV"),"Erreur Magie")))),"Erreur"))</f>
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="Y25" s="62"/>
       <c r="Z25" s="62"/>
@@ -10065,7 +10065,7 @@
       <formula>"Force"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations disablePrompts="1" count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S7" xr:uid="{F4ED68C8-9DBD-4E63-80C7-B89DC5A479EB}">
       <formula1>$P$5:$P$20</formula1>
     </dataValidation>
@@ -10089,7 +10089,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F49B2BA0-7E1A-424B-9903-B90A3FC81D08}">
           <x14:formula1>
             <xm:f>Données!$A$2:$A$3</xm:f>

</xml_diff>